<commit_message>
feat: render, update guide, and fix datasets - render the module to update the website - update the Git guide - change rstudio window illustration - fix dataset UINRIL & UBL
</commit_message>
<xml_diff>
--- a/Data UINRIL & UBL.xlsx
+++ b/Data UINRIL & UBL.xlsx
@@ -14,61 +14,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
-    <t xml:space="preserve">Nomor.urut</t>
+    <t xml:space="preserve">nomor_urut</t>
   </si>
   <si>
-    <t xml:space="preserve">Jenis.Kelamin</t>
+    <t xml:space="preserve">jenis_kelamin</t>
   </si>
   <si>
-    <t xml:space="preserve">Umur</t>
+    <t xml:space="preserve">umur</t>
   </si>
   <si>
-    <t xml:space="preserve">Fakultas</t>
+    <t xml:space="preserve">fakultas</t>
   </si>
   <si>
-    <t xml:space="preserve">Prodi</t>
+    <t xml:space="preserve">prodi</t>
   </si>
   <si>
-    <t xml:space="preserve">Tingkat.Semester</t>
+    <t xml:space="preserve">tingkat_semester</t>
   </si>
   <si>
-    <t xml:space="preserve">Uang.Saku</t>
+    <t xml:space="preserve">uang_saku</t>
   </si>
   <si>
-    <t xml:space="preserve">kepemilikan.mobil</t>
+    <t xml:space="preserve">kepemilikan_mobil</t>
   </si>
   <si>
-    <t xml:space="preserve">kepemilikan.motor</t>
+    <t xml:space="preserve">kepemilikan_motor</t>
   </si>
   <si>
-    <t xml:space="preserve">kepemilikan.sepeda</t>
+    <t xml:space="preserve">kepemilikan_sepeda</t>
   </si>
   <si>
-    <t xml:space="preserve">kendaraan.utama</t>
+    <t xml:space="preserve">kendaraan_utama</t>
   </si>
   <si>
-    <t xml:space="preserve">jenis.tempat.tinggal</t>
+    <t xml:space="preserve">jenis_tempat_tinggal</t>
   </si>
   <si>
     <t xml:space="preserve">jarak</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Selasa</t>
+    <t xml:space="preserve">jumlah_perjalanan_selasa</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Rabu</t>
+    <t xml:space="preserve">jumlah_perjalanan_rabu</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Kamis</t>
+    <t xml:space="preserve">jumlah_perjalanan_kamis</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Jumat</t>
+    <t xml:space="preserve">jumlah_perjalanan_jumat</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Sabtu</t>
+    <t xml:space="preserve">jumlah_perjalanan_sabtu</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah.perjalanan.Ahad</t>
+    <t xml:space="preserve">jumlah_perjalanan_ahad</t>
   </si>
   <si>
     <t xml:space="preserve">Laki-laki</t>

</xml_diff>